<commit_message>
DAL finished for 10/1/2015
</commit_message>
<xml_diff>
--- a/Daily Activity Log - Iteration 2 - Alex and Glenn.xlsx
+++ b/Daily Activity Log - Iteration 2 - Alex and Glenn.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="35">
   <si>
     <t>Hours Worked Per Day</t>
   </si>
@@ -42,24 +42,24 @@
     <t>    Send email confirmation after reminder is created</t>
   </si>
   <si>
+    <t>Alexander</t>
+  </si>
+  <si>
     <t>    Upload picture (optional)</t>
   </si>
   <si>
+    <t>Glenn</t>
+  </si>
+  <si>
     <t>    Send email confirmation after account is created</t>
   </si>
   <si>
     <t>Edit your reminders</t>
   </si>
   <si>
-    <t>Alexander</t>
-  </si>
-  <si>
     <t>Fixed: Glenn</t>
   </si>
   <si>
-    <t>*</t>
-  </si>
-  <si>
     <t>Mark the added row green for 3 seconds.</t>
   </si>
   <si>
@@ -106,9 +106,6 @@
   </si>
   <si>
     <t>    Reminder text</t>
-  </si>
-  <si>
-    <t>Moved to 2nd Iteration</t>
   </si>
   <si>
     <t>    Date for first email</t>
@@ -182,7 +179,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -197,8 +194,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFCCFFFF"/>
+        <fgColor rgb="FF9999FF"/>
+        <bgColor rgb="FFCC99FF"/>
       </patternFill>
     </fill>
     <fill>
@@ -209,20 +206,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF9999FF"/>
-        <bgColor rgb="FFCC99FF"/>
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFCCFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor rgb="FFFCD5B5"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -389,15 +380,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="168" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -413,7 +408,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -421,11 +416,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -521,31 +512,29 @@
   <dimension ref="A1:AA26"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F27" activeCellId="0" sqref="F27"/>
+      <selection pane="topLeft" activeCell="R17" activeCellId="0" sqref="R17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="64.2397959183674"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="4.45408163265306"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="63.5816326530612"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="4.32142857142857"/>
     <col collapsed="false" hidden="false" max="9" min="8" style="0" width="3.51020408163265"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="3.37244897959184"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="3.51020408163265"/>
-    <col collapsed="false" hidden="false" max="13" min="12" style="0" width="3.64285714285714"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="3.51020408163265"/>
+    <col collapsed="false" hidden="false" max="14" min="11" style="0" width="3.51020408163265"/>
     <col collapsed="false" hidden="false" max="15" min="15" style="0" width="3.23979591836735"/>
     <col collapsed="false" hidden="false" max="19" min="16" style="0" width="3.51020408163265"/>
-    <col collapsed="false" hidden="false" max="21" min="20" style="0" width="3.78061224489796"/>
+    <col collapsed="false" hidden="false" max="21" min="20" style="0" width="3.64285714285714"/>
     <col collapsed="false" hidden="true" max="22" min="22" style="0" width="0"/>
     <col collapsed="false" hidden="false" max="23" min="23" style="0" width="3.37244897959184"/>
     <col collapsed="false" hidden="false" max="26" min="24" style="0" width="3.51020408163265"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="25.6479591836735"/>
-    <col collapsed="false" hidden="false" max="1025" min="28" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="25.3775510204082"/>
+    <col collapsed="false" hidden="false" max="1025" min="28" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="26.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -623,13 +612,19 @@
         <v>7</v>
       </c>
       <c r="B3" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="C3" s="11"/>
-      <c r="D3" s="12"/>
+        <v>0</v>
+      </c>
+      <c r="C3" s="11" t="n">
+        <v>42276</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="E3" s="13"/>
       <c r="F3" s="14"/>
-      <c r="G3" s="10"/>
+      <c r="G3" s="10" t="n">
+        <v>1</v>
+      </c>
       <c r="H3" s="10"/>
       <c r="I3" s="10"/>
       <c r="J3" s="10"/>
@@ -642,13 +637,17 @@
     </row>
     <row r="4" customFormat="false" ht="16.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B4" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="C4" s="11"/>
-      <c r="D4" s="15"/>
+        <v>0</v>
+      </c>
+      <c r="C4" s="11" t="n">
+        <v>42278</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>10</v>
+      </c>
       <c r="E4" s="13"/>
       <c r="F4" s="14"/>
       <c r="G4" s="10"/>
@@ -664,13 +663,17 @@
     </row>
     <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="9" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B5" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="C5" s="11"/>
-      <c r="D5" s="15"/>
+        <v>0</v>
+      </c>
+      <c r="C5" s="11" t="n">
+        <v>42276</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>8</v>
+      </c>
       <c r="E5" s="13"/>
       <c r="F5" s="14"/>
       <c r="G5" s="10"/>
@@ -686,22 +689,24 @@
     </row>
     <row r="6" customFormat="false" ht="16.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="16" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B6" s="17" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6" s="18" t="n">
         <v>42264</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E6" s="19" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F6" s="20"/>
-      <c r="G6" s="17"/>
+      <c r="G6" s="17" t="n">
+        <v>2</v>
+      </c>
       <c r="H6" s="17"/>
       <c r="I6" s="17"/>
       <c r="J6" s="17"/>
@@ -711,28 +716,25 @@
       <c r="N6" s="17"/>
       <c r="O6" s="17"/>
       <c r="P6" s="17"/>
-      <c r="Q6" s="0" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="7" customFormat="false" ht="17.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="21" t="s">
         <v>14</v>
       </c>
       <c r="B7" s="17" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" s="18" t="n">
+        <v>42276</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="19"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="17" t="n">
         <v>1</v>
       </c>
-      <c r="C7" s="18" t="n">
-        <v>42264</v>
-      </c>
-      <c r="D7" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" s="20"/>
-      <c r="G7" s="17"/>
       <c r="H7" s="17"/>
       <c r="I7" s="17"/>
       <c r="J7" s="17"/>
@@ -742,19 +744,20 @@
       <c r="N7" s="17"/>
       <c r="O7" s="17"/>
       <c r="P7" s="17"/>
-      <c r="Q7" s="0" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="8" customFormat="false" ht="13.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="9" t="s">
         <v>15</v>
       </c>
       <c r="B8" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="C8" s="11"/>
-      <c r="D8" s="15"/>
+        <v>0</v>
+      </c>
+      <c r="C8" s="11" t="n">
+        <v>42276</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>8</v>
+      </c>
       <c r="E8" s="13"/>
       <c r="F8" s="14"/>
       <c r="G8" s="10"/>
@@ -768,15 +771,19 @@
       <c r="O8" s="10"/>
       <c r="P8" s="10"/>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="9" t="s">
         <v>16</v>
       </c>
       <c r="B9" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="C9" s="11"/>
-      <c r="D9" s="15"/>
+        <v>0</v>
+      </c>
+      <c r="C9" s="11" t="n">
+        <v>42276</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>8</v>
+      </c>
       <c r="E9" s="13"/>
       <c r="F9" s="14"/>
       <c r="G9" s="10"/>
@@ -790,18 +797,24 @@
       <c r="O9" s="10"/>
       <c r="P9" s="10"/>
     </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="22" t="s">
         <v>14</v>
       </c>
       <c r="B10" s="23" t="n">
-        <v>1</v>
-      </c>
-      <c r="C10" s="24"/>
-      <c r="D10" s="24"/>
+        <v>0</v>
+      </c>
+      <c r="C10" s="18" t="n">
+        <v>42276</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>10</v>
+      </c>
       <c r="E10" s="24"/>
       <c r="F10" s="24"/>
-      <c r="G10" s="24"/>
+      <c r="G10" s="23" t="n">
+        <v>1</v>
+      </c>
       <c r="H10" s="24"/>
       <c r="I10" s="24"/>
       <c r="J10" s="24"/>
@@ -812,267 +825,290 @@
       <c r="O10" s="24"/>
       <c r="P10" s="24"/>
     </row>
-    <row r="11" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="9" t="s">
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="25"/>
-      <c r="C11" s="26"/>
-      <c r="D11" s="27"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="28"/>
-      <c r="G11" s="28"/>
-      <c r="H11" s="28"/>
-      <c r="I11" s="28"/>
-      <c r="J11" s="28"/>
-      <c r="K11" s="28"/>
-      <c r="L11" s="28"/>
-      <c r="M11" s="28"/>
-      <c r="N11" s="28"/>
-      <c r="O11" s="28"/>
-      <c r="P11" s="28"/>
-    </row>
-    <row r="12" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="9" t="s">
+      <c r="B11" s="26" t="n">
+        <v>0</v>
+      </c>
+      <c r="C11" s="27"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="29"/>
+      <c r="G11" s="29"/>
+      <c r="H11" s="29"/>
+      <c r="I11" s="29"/>
+      <c r="J11" s="29"/>
+      <c r="K11" s="29"/>
+      <c r="L11" s="29"/>
+      <c r="M11" s="29"/>
+      <c r="N11" s="29"/>
+      <c r="O11" s="29"/>
+      <c r="P11" s="29"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="25"/>
-      <c r="C12" s="26"/>
-      <c r="D12" s="27"/>
-      <c r="E12" s="28"/>
-      <c r="F12" s="28"/>
-      <c r="G12" s="28"/>
-      <c r="H12" s="28"/>
-      <c r="I12" s="28"/>
-      <c r="J12" s="28"/>
-      <c r="K12" s="28"/>
-      <c r="L12" s="28"/>
-      <c r="M12" s="28"/>
-      <c r="N12" s="28"/>
-      <c r="O12" s="28"/>
-      <c r="P12" s="28"/>
-    </row>
-    <row r="13" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="9" t="s">
+      <c r="B12" s="26" t="n">
+        <v>0</v>
+      </c>
+      <c r="C12" s="27"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="29"/>
+      <c r="G12" s="29"/>
+      <c r="H12" s="29"/>
+      <c r="I12" s="29"/>
+      <c r="J12" s="29"/>
+      <c r="K12" s="29"/>
+      <c r="L12" s="29"/>
+      <c r="M12" s="29"/>
+      <c r="N12" s="29"/>
+      <c r="O12" s="29"/>
+      <c r="P12" s="29"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="25"/>
-      <c r="C13" s="26"/>
-      <c r="D13" s="27"/>
-      <c r="E13" s="28"/>
-      <c r="F13" s="28"/>
-      <c r="G13" s="28"/>
-      <c r="H13" s="28"/>
-      <c r="I13" s="28"/>
-      <c r="J13" s="28"/>
-      <c r="K13" s="28"/>
-      <c r="L13" s="28"/>
-      <c r="M13" s="28"/>
-      <c r="N13" s="28"/>
-      <c r="O13" s="28"/>
-      <c r="P13" s="28"/>
-    </row>
-    <row r="14" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="9" t="s">
+      <c r="B13" s="26" t="n">
+        <v>0</v>
+      </c>
+      <c r="C13" s="27"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="29"/>
+      <c r="F13" s="29"/>
+      <c r="G13" s="29"/>
+      <c r="H13" s="29"/>
+      <c r="I13" s="29"/>
+      <c r="J13" s="29"/>
+      <c r="K13" s="29"/>
+      <c r="L13" s="29"/>
+      <c r="M13" s="29"/>
+      <c r="N13" s="29"/>
+      <c r="O13" s="29"/>
+      <c r="P13" s="29"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="25"/>
-      <c r="C14" s="26"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="28"/>
-      <c r="F14" s="28"/>
-      <c r="G14" s="28"/>
-      <c r="H14" s="28"/>
-      <c r="I14" s="28"/>
-      <c r="J14" s="28"/>
-      <c r="K14" s="28"/>
-      <c r="L14" s="28"/>
-      <c r="M14" s="28"/>
-      <c r="N14" s="28"/>
-      <c r="O14" s="28"/>
-      <c r="P14" s="28"/>
-    </row>
-    <row r="15" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="9" t="s">
+      <c r="B14" s="26" t="n">
+        <v>0</v>
+      </c>
+      <c r="C14" s="27"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="29"/>
+      <c r="F14" s="29"/>
+      <c r="G14" s="29"/>
+      <c r="H14" s="29"/>
+      <c r="I14" s="29"/>
+      <c r="J14" s="29"/>
+      <c r="K14" s="29"/>
+      <c r="L14" s="29"/>
+      <c r="M14" s="29"/>
+      <c r="N14" s="29"/>
+      <c r="O14" s="29"/>
+      <c r="P14" s="29"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="25"/>
-      <c r="C15" s="26"/>
-      <c r="D15" s="27"/>
-      <c r="E15" s="28"/>
-      <c r="F15" s="28"/>
-      <c r="G15" s="28"/>
-      <c r="H15" s="28"/>
-      <c r="I15" s="28"/>
-      <c r="J15" s="28"/>
-      <c r="K15" s="28"/>
-      <c r="L15" s="28"/>
-      <c r="M15" s="28"/>
-      <c r="N15" s="28"/>
-      <c r="O15" s="28"/>
-      <c r="P15" s="28"/>
-    </row>
-    <row r="16" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="9" t="s">
+      <c r="B15" s="26" t="n">
+        <v>0</v>
+      </c>
+      <c r="C15" s="27"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="29"/>
+      <c r="F15" s="29"/>
+      <c r="G15" s="29"/>
+      <c r="H15" s="29"/>
+      <c r="I15" s="29"/>
+      <c r="J15" s="29"/>
+      <c r="K15" s="29"/>
+      <c r="L15" s="29"/>
+      <c r="M15" s="29"/>
+      <c r="N15" s="29"/>
+      <c r="O15" s="29"/>
+      <c r="P15" s="29"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="25"/>
-      <c r="C16" s="26"/>
-      <c r="D16" s="27"/>
-      <c r="E16" s="28"/>
-      <c r="F16" s="28"/>
-      <c r="G16" s="28"/>
-      <c r="H16" s="28"/>
-      <c r="I16" s="28"/>
-      <c r="J16" s="28"/>
-      <c r="K16" s="28"/>
-      <c r="L16" s="28"/>
-      <c r="M16" s="28"/>
-      <c r="N16" s="28"/>
-      <c r="O16" s="28"/>
-      <c r="P16" s="28"/>
-      <c r="AA16" s="29" t="s">
+      <c r="B16" s="26" t="n">
+        <v>0</v>
+      </c>
+      <c r="C16" s="27"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="29"/>
+      <c r="F16" s="29"/>
+      <c r="G16" s="29"/>
+      <c r="H16" s="29"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="29"/>
+      <c r="K16" s="29"/>
+      <c r="L16" s="29"/>
+      <c r="M16" s="29"/>
+      <c r="N16" s="29"/>
+      <c r="O16" s="29"/>
+      <c r="P16" s="29"/>
+      <c r="AA16" s="30" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="9" t="s">
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="B17" s="25"/>
-      <c r="C17" s="26"/>
-      <c r="D17" s="27"/>
-      <c r="E17" s="28"/>
-      <c r="F17" s="28"/>
-      <c r="G17" s="28"/>
-      <c r="H17" s="28"/>
-      <c r="I17" s="28"/>
-      <c r="J17" s="28"/>
-      <c r="K17" s="28"/>
-      <c r="L17" s="28"/>
-      <c r="M17" s="28"/>
-      <c r="N17" s="28"/>
-      <c r="O17" s="28"/>
-      <c r="P17" s="28"/>
-      <c r="AA17" s="30" t="s">
+      <c r="B17" s="26" t="n">
+        <v>0</v>
+      </c>
+      <c r="C17" s="27"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="29"/>
+      <c r="F17" s="29"/>
+      <c r="G17" s="29"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="29"/>
+      <c r="K17" s="29"/>
+      <c r="L17" s="29"/>
+      <c r="M17" s="29"/>
+      <c r="N17" s="29"/>
+      <c r="O17" s="29"/>
+      <c r="P17" s="29"/>
+      <c r="AA17" s="31" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="9" t="s">
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="B18" s="25"/>
-      <c r="C18" s="26"/>
-      <c r="D18" s="27"/>
-      <c r="E18" s="28"/>
-      <c r="F18" s="28"/>
-      <c r="G18" s="28"/>
-      <c r="H18" s="28"/>
-      <c r="I18" s="28"/>
-      <c r="J18" s="28"/>
-      <c r="K18" s="28"/>
-      <c r="L18" s="28"/>
-      <c r="M18" s="28"/>
-      <c r="N18" s="28"/>
-      <c r="O18" s="28"/>
-      <c r="P18" s="28"/>
-      <c r="AA18" s="31" t="s">
+      <c r="B18" s="26" t="n">
+        <v>0</v>
+      </c>
+      <c r="C18" s="27"/>
+      <c r="D18" s="28"/>
+      <c r="E18" s="29"/>
+      <c r="F18" s="29"/>
+      <c r="G18" s="29"/>
+      <c r="H18" s="29"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="29"/>
+      <c r="K18" s="29"/>
+      <c r="L18" s="29"/>
+      <c r="M18" s="29"/>
+      <c r="N18" s="29"/>
+      <c r="O18" s="29"/>
+      <c r="P18" s="29"/>
+      <c r="AA18" s="32" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="9" t="s">
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="B19" s="25"/>
-      <c r="C19" s="26"/>
-      <c r="D19" s="27"/>
-      <c r="E19" s="28"/>
-      <c r="F19" s="28"/>
-      <c r="G19" s="28"/>
-      <c r="H19" s="28"/>
-      <c r="I19" s="28"/>
-      <c r="J19" s="28"/>
-      <c r="K19" s="28"/>
-      <c r="L19" s="28"/>
-      <c r="M19" s="28"/>
-      <c r="N19" s="28"/>
-      <c r="O19" s="28"/>
-      <c r="P19" s="28"/>
-      <c r="AA19" s="32" t="s">
+      <c r="B19" s="26" t="n">
+        <v>0</v>
+      </c>
+      <c r="C19" s="27"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="29"/>
+      <c r="F19" s="29"/>
+      <c r="G19" s="29"/>
+      <c r="H19" s="29"/>
+      <c r="I19" s="29"/>
+      <c r="J19" s="29"/>
+      <c r="K19" s="29"/>
+      <c r="L19" s="29"/>
+      <c r="M19" s="29"/>
+      <c r="N19" s="29"/>
+      <c r="O19" s="29"/>
+      <c r="P19" s="29"/>
+      <c r="AA19" s="33" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="9" t="s">
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="25"/>
-      <c r="C20" s="26"/>
-      <c r="D20" s="27"/>
-      <c r="E20" s="28"/>
-      <c r="F20" s="28"/>
-      <c r="G20" s="28"/>
-      <c r="H20" s="28"/>
-      <c r="I20" s="28"/>
-      <c r="J20" s="28"/>
-      <c r="K20" s="28"/>
-      <c r="L20" s="28"/>
-      <c r="M20" s="28"/>
-      <c r="N20" s="28"/>
-      <c r="O20" s="28"/>
-      <c r="P20" s="28"/>
-      <c r="AA20" s="33" t="s">
+      <c r="B20" s="26" t="n">
+        <v>0</v>
+      </c>
+      <c r="C20" s="27"/>
+      <c r="D20" s="28"/>
+      <c r="E20" s="29"/>
+      <c r="F20" s="29"/>
+      <c r="G20" s="29"/>
+      <c r="H20" s="29"/>
+      <c r="I20" s="29"/>
+      <c r="J20" s="29"/>
+      <c r="K20" s="29"/>
+      <c r="L20" s="29"/>
+      <c r="M20" s="29"/>
+      <c r="N20" s="29"/>
+      <c r="O20" s="29"/>
+      <c r="P20" s="29"/>
+      <c r="AA20" s="34"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="25" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="9" t="s">
+      <c r="B21" s="26" t="n">
+        <v>0</v>
+      </c>
+      <c r="C21" s="27"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="29"/>
+      <c r="F21" s="29"/>
+      <c r="G21" s="29"/>
+      <c r="H21" s="29"/>
+      <c r="I21" s="29"/>
+      <c r="J21" s="29"/>
+      <c r="K21" s="29"/>
+      <c r="L21" s="29"/>
+      <c r="M21" s="29"/>
+      <c r="N21" s="29"/>
+      <c r="O21" s="29"/>
+      <c r="P21" s="29"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="B21" s="25"/>
-      <c r="C21" s="26"/>
-      <c r="D21" s="27"/>
-      <c r="E21" s="28"/>
-      <c r="F21" s="28"/>
-      <c r="G21" s="28"/>
-      <c r="H21" s="28"/>
-      <c r="I21" s="28"/>
-      <c r="J21" s="28"/>
-      <c r="K21" s="28"/>
-      <c r="L21" s="28"/>
-      <c r="M21" s="28"/>
-      <c r="N21" s="28"/>
-      <c r="O21" s="28"/>
-      <c r="P21" s="28"/>
-      <c r="AA21" s="34"/>
-    </row>
-    <row r="22" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="B22" s="25"/>
-      <c r="C22" s="26"/>
-      <c r="D22" s="27"/>
-      <c r="E22" s="28"/>
-      <c r="F22" s="28"/>
-      <c r="G22" s="28"/>
-      <c r="H22" s="28"/>
-      <c r="I22" s="28"/>
-      <c r="J22" s="28"/>
-      <c r="K22" s="28"/>
-      <c r="L22" s="28"/>
-      <c r="M22" s="28"/>
-      <c r="N22" s="28"/>
-      <c r="O22" s="28"/>
-      <c r="P22" s="28"/>
+      <c r="B22" s="26" t="n">
+        <v>0</v>
+      </c>
+      <c r="C22" s="27"/>
+      <c r="D22" s="28"/>
+      <c r="E22" s="29"/>
+      <c r="F22" s="29"/>
+      <c r="G22" s="29"/>
+      <c r="H22" s="29"/>
+      <c r="I22" s="29"/>
+      <c r="J22" s="29"/>
+      <c r="K22" s="29"/>
+      <c r="L22" s="29"/>
+      <c r="M22" s="29"/>
+      <c r="N22" s="29"/>
+      <c r="O22" s="29"/>
+      <c r="P22" s="29"/>
     </row>
     <row r="23" customFormat="false" ht="24.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="B23" s="35"/>
+        <v>32</v>
+      </c>
+      <c r="B23" s="35" t="n">
+        <v>0</v>
+      </c>
       <c r="C23" s="36"/>
       <c r="D23" s="37"/>
       <c r="E23" s="24"/>
@@ -1088,29 +1124,33 @@
       <c r="O23" s="24"/>
       <c r="P23" s="24"/>
     </row>
-    <row r="24" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="B24" s="25"/>
-      <c r="C24" s="26"/>
-      <c r="D24" s="27"/>
-      <c r="E24" s="28"/>
-      <c r="F24" s="28"/>
-      <c r="G24" s="28"/>
-      <c r="H24" s="28"/>
-      <c r="I24" s="28"/>
-      <c r="J24" s="28"/>
-      <c r="K24" s="28"/>
-      <c r="L24" s="28"/>
-      <c r="M24" s="28"/>
-      <c r="N24" s="28"/>
-      <c r="O24" s="28"/>
-      <c r="P24" s="28"/>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="B24" s="26" t="n">
+        <v>0</v>
+      </c>
+      <c r="C24" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="D24" s="28"/>
+      <c r="E24" s="29"/>
+      <c r="F24" s="29"/>
+      <c r="G24" s="29"/>
+      <c r="H24" s="29"/>
+      <c r="I24" s="29"/>
+      <c r="J24" s="29"/>
+      <c r="K24" s="29"/>
+      <c r="L24" s="29"/>
+      <c r="M24" s="29"/>
+      <c r="N24" s="29"/>
+      <c r="O24" s="29"/>
+      <c r="P24" s="29"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E26" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added durations to DAL
</commit_message>
<xml_diff>
--- a/Daily Activity Log - Iteration 2 - Alex and Glenn.xlsx
+++ b/Daily Activity Log - Iteration 2 - Alex and Glenn.xlsx
@@ -279,7 +279,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="41">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -429,6 +429,18 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -512,29 +524,25 @@
   <dimension ref="A1:AA26"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="R17" activeCellId="0" sqref="R17"/>
+      <selection pane="topLeft" activeCell="F26" activeCellId="0" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="63.5816326530612"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="4.32142857142857"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="62.7704081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="4.18367346938776"/>
     <col collapsed="false" hidden="false" max="9" min="8" style="0" width="3.51020408163265"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="3.37244897959184"/>
     <col collapsed="false" hidden="false" max="14" min="11" style="0" width="3.51020408163265"/>
     <col collapsed="false" hidden="false" max="15" min="15" style="0" width="3.23979591836735"/>
-    <col collapsed="false" hidden="false" max="19" min="16" style="0" width="3.51020408163265"/>
-    <col collapsed="false" hidden="false" max="21" min="20" style="0" width="3.64285714285714"/>
+    <col collapsed="false" hidden="false" max="21" min="16" style="0" width="3.51020408163265"/>
     <col collapsed="false" hidden="true" max="22" min="22" style="0" width="0"/>
     <col collapsed="false" hidden="false" max="23" min="23" style="0" width="3.37244897959184"/>
     <col collapsed="false" hidden="false" max="26" min="24" style="0" width="3.51020408163265"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="25.3775510204082"/>
-    <col collapsed="false" hidden="false" max="1025" min="28" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="25.1071428571429"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="26.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -612,7 +620,7 @@
         <v>7</v>
       </c>
       <c r="B3" s="10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3" s="11" t="n">
         <v>42276</v>
@@ -640,7 +648,7 @@
         <v>9</v>
       </c>
       <c r="B4" s="10" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C4" s="11" t="n">
         <v>42278</v>
@@ -666,7 +674,7 @@
         <v>11</v>
       </c>
       <c r="B5" s="10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5" s="11" t="n">
         <v>42276</v>
@@ -692,7 +700,7 @@
         <v>12</v>
       </c>
       <c r="B6" s="17" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C6" s="18" t="n">
         <v>42264</v>
@@ -722,7 +730,7 @@
         <v>14</v>
       </c>
       <c r="B7" s="17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7" s="18" t="n">
         <v>42276</v>
@@ -750,7 +758,7 @@
         <v>15</v>
       </c>
       <c r="B8" s="10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C8" s="11" t="n">
         <v>42276</v>
@@ -776,7 +784,7 @@
         <v>16</v>
       </c>
       <c r="B9" s="10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C9" s="11" t="n">
         <v>42276</v>
@@ -802,7 +810,7 @@
         <v>14</v>
       </c>
       <c r="B10" s="23" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C10" s="18" t="n">
         <v>42276</v>
@@ -1124,29 +1132,29 @@
       <c r="O23" s="24"/>
       <c r="P23" s="24"/>
     </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="25" t="s">
+    <row r="24" customFormat="false" ht="28.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="B24" s="26" t="n">
-        <v>0</v>
-      </c>
-      <c r="C24" s="27" t="s">
+      <c r="B24" s="38" t="n">
+        <v>2</v>
+      </c>
+      <c r="C24" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="D24" s="28"/>
-      <c r="E24" s="29"/>
-      <c r="F24" s="29"/>
-      <c r="G24" s="29"/>
-      <c r="H24" s="29"/>
-      <c r="I24" s="29"/>
-      <c r="J24" s="29"/>
-      <c r="K24" s="29"/>
-      <c r="L24" s="29"/>
-      <c r="M24" s="29"/>
-      <c r="N24" s="29"/>
-      <c r="O24" s="29"/>
-      <c r="P24" s="29"/>
+      <c r="D24" s="40"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
+      <c r="H24" s="13"/>
+      <c r="I24" s="13"/>
+      <c r="J24" s="13"/>
+      <c r="K24" s="13"/>
+      <c r="L24" s="13"/>
+      <c r="M24" s="13"/>
+      <c r="N24" s="13"/>
+      <c r="O24" s="13"/>
+      <c r="P24" s="13"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E26" s="0" t="s">

</xml_diff>